<commit_message>
Putting Things together 2
- Updated the Student and Committee Menu
</commit_message>
<xml_diff>
--- a/data/student_list.xlsx
+++ b/data/student_list.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive - Nanyang Technological University\Y2S1\SC2002\CampManagement\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{47BE22ED-BBDB-493F-81B6-3430F46B512A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994F0784-DE76-4E51-8154-464D1E0F0E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="11295" windowWidth="21600" xWindow="4605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="2460"/>
+    <workbookView xWindow="4605" yWindow="2460" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -71,9 +71,6 @@
     <t xml:space="preserve">LEE </t>
   </si>
   <si>
-    <t xml:space="preserve">LIU </t>
-  </si>
-  <si>
     <t>RAWAL</t>
   </si>
   <si>
@@ -146,14 +143,13 @@
     <t>LIU</t>
   </si>
   <si>
-    <t>1</t>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -203,20 +199,20 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -233,10 +229,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -271,7 +267,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -306,7 +302,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -400,21 +396,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -431,7 +427,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -483,25 +479,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.5703125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="36.7109375" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="false"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -512,16 +508,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -529,16 +525,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -546,16 +545,19 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -563,16 +565,19 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -580,16 +585,19 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -597,16 +605,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -614,16 +625,19 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -631,16 +645,19 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -648,16 +665,19 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -665,68 +685,77 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{B663E933-92D6-47AE-9545-627F61C39D32}"/>
-    <hyperlink r:id="rId2" ref="B3" xr:uid="{91C33AD5-35F2-4A3A-959A-C87C2162E9B9}"/>
-    <hyperlink r:id="rId3" ref="B4" xr:uid="{3361E6EC-8183-4CC2-9EB5-4D8406720EFD}"/>
-    <hyperlink r:id="rId4" ref="B5" xr:uid="{955E528D-1008-47EA-A35C-104EB72DF944}"/>
-    <hyperlink r:id="rId5" ref="B6" xr:uid="{54EF69E7-4E62-469D-AA1E-4618A065A189}"/>
-    <hyperlink r:id="rId6" ref="B7" xr:uid="{7254179A-C06A-483F-AAD0-CC3AAA78DFAB}"/>
-    <hyperlink r:id="rId7" ref="B8" xr:uid="{4F024CCC-B278-4021-BDF8-EBF854AA15C1}"/>
-    <hyperlink r:id="rId8" ref="B9" xr:uid="{4BC2904C-82AC-418F-8A40-8AEE365A78F6}"/>
-    <hyperlink r:id="rId9" ref="B10" xr:uid="{D76D6340-A367-4E32-ABF4-257D40F0ED14}"/>
-    <hyperlink r:id="rId10" ref="B11" xr:uid="{4E0422A0-CAA4-4F75-82E6-A434E940A6B7}"/>
-    <hyperlink r:id="rId11" ref="B12" xr:uid="{3F90C71F-80BE-4B48-977D-3B37A5AD0B30}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B663E933-92D6-47AE-9545-627F61C39D32}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{91C33AD5-35F2-4A3A-959A-C87C2162E9B9}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{3361E6EC-8183-4CC2-9EB5-4D8406720EFD}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{955E528D-1008-47EA-A35C-104EB72DF944}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{54EF69E7-4E62-469D-AA1E-4618A065A189}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{7254179A-C06A-483F-AAD0-CC3AAA78DFAB}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{4F024CCC-B278-4021-BDF8-EBF854AA15C1}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{4BC2904C-82AC-418F-8A40-8AEE365A78F6}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{D76D6340-A367-4E32-ABF4-257D40F0ED14}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{4E0422A0-CAA4-4F75-82E6-A434E940A6B7}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{3F90C71F-80BE-4B48-977D-3B37A5AD0B30}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId12"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Putting Things together 3
- Changes made to the user data system to make sure that data is saved within the instance
</commit_message>
<xml_diff>
--- a/data/student_list.xlsx
+++ b/data/student_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive - Nanyang Technological University\Y2S1\SC2002\CampManagement\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994F0784-DE76-4E51-8154-464D1E0F0E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F0A270-AAC4-4752-8990-0D701B43A4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4605" yWindow="2460" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -44,18 +44,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t xml:space="preserve">CHERN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRANDON </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALVIN </t>
-  </si>
-  <si>
     <t>CHAN</t>
   </si>
   <si>
@@ -68,9 +56,6 @@
     <t>ERNEST</t>
   </si>
   <si>
-    <t xml:space="preserve">LEE </t>
-  </si>
-  <si>
     <t>RAWAL</t>
   </si>
   <si>
@@ -144,6 +129,24 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>CHERN</t>
+  </si>
+  <si>
+    <t>KOH</t>
+  </si>
+  <si>
+    <t>BRANDON</t>
+  </si>
+  <si>
+    <t>CALVIN</t>
+  </si>
+  <si>
+    <t>LEE</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,236 +511,236 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>